<commit_message>
Updated LC.xlsx with more problems
</commit_message>
<xml_diff>
--- a/LC.xlsx
+++ b/LC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameer/Desktop/goApps/LC-random/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A80AB-28F3-DD46-AF8B-9B5C9B3AEA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9511949F-9EE6-154C-8B07-C02B6E515F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
   <si>
     <t>PROBLEM</t>
   </si>
@@ -137,6 +137,183 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/trapping-rain-water/</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/</t>
+  </si>
+  <si>
+    <t>Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-repeating-character-replacement/</t>
+  </si>
+  <si>
+    <t>Permutation In String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutation-in-string/</t>
+  </si>
+  <si>
+    <t>Sliding Window Maximum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sliding-window-maximum/</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-parentheses/</t>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
+  </si>
+  <si>
+    <t>Generate Parentheses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/generate-parentheses/</t>
+  </si>
+  <si>
+    <t>Car Fleet</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/car-fleet/</t>
+  </si>
+  <si>
+    <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/koko-eating-bananas/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t>Find Minimum In Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/median-of-two-sorted-arrays/</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>Merge K Sorted Lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-nth-node-from-end-of-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-k-sorted-lists/</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/</t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>Count Good Nodes In Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-good-nodes-in-binary-tree/</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-maximum-path-sum/</t>
+  </si>
+  <si>
+    <t>Implement Trie Prefix Tree</t>
+  </si>
+  <si>
+    <t>Tries</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>Word Search II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-search-ii/</t>
+  </si>
+  <si>
+    <t>Kth Largest Element In a Stream</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-largest-element-in-a-stream/</t>
+  </si>
+  <si>
+    <t>Task Scheduler</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/task-scheduler/</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>Rotting Oranges</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotting-oranges/</t>
   </si>
 </sst>
 </file>
@@ -697,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -911,6 +1088,370 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -924,6 +1465,12 @@
     <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{3A23853C-06B6-5747-B0DF-C3337DA24152}"/>
+    <hyperlink ref="B22" r:id="rId13" xr:uid="{1FACE5D8-1CE3-9A43-856C-CFA784FCF3A4}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{DF091EBE-0ACC-984C-99C7-C73BADA34EED}"/>
+    <hyperlink ref="B33" r:id="rId15" xr:uid="{50CD7341-9A1A-9B40-8C5C-2F8A99FD3596}"/>
+    <hyperlink ref="B34" r:id="rId16" xr:uid="{BB50B45F-FEF3-B94D-B88D-12B26DB25690}"/>
+    <hyperlink ref="B38" r:id="rId17" xr:uid="{9F919F12-5A2F-884E-8F9E-8256B3D82DF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>